<commit_message>
Updated documentation and TODO
</commit_message>
<xml_diff>
--- a/Workbooks/repo-datastore.xlsx
+++ b/Workbooks/repo-datastore.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Repos\Private\excel-data-store\Workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Repos\Public\excel-data-store\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01BE173-D365-47D1-89A8-7A75DEBE1F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5947F925-623D-4411-8D06-9E8A9D85055D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28695" yWindow="8940" windowWidth="21600" windowHeight="6480" activeTab="3" xr2:uid="{69AEAB45-AF6A-4548-B086-2C108EB58740}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{69AEAB45-AF6A-4548-B086-2C108EB58740}"/>
   </bookViews>
   <sheets>
     <sheet name="Store" sheetId="1" r:id="rId1"/>
     <sheet name="Keys" sheetId="2" r:id="rId2"/>
     <sheet name="Fields" sheetId="3" r:id="rId3"/>
     <sheet name="Values" sheetId="4" r:id="rId4"/>
-    <sheet name="Commits" sheetId="5" r:id="rId5"/>
-    <sheet name="Maps" sheetId="6" r:id="rId6"/>
-    <sheet name="Tables" sheetId="7" r:id="rId7"/>
+    <sheet name="ValuesHistory" sheetId="8" r:id="rId5"/>
+    <sheet name="Commits" sheetId="5" r:id="rId6"/>
+    <sheet name="Maps" sheetId="6" r:id="rId7"/>
+    <sheet name="Tables" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Fields!$A$1:$G$11</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1271" uniqueCount="477">
   <si>
     <t>Key</t>
   </si>
@@ -1449,6 +1450,33 @@
   </si>
   <si>
     <t>Book3§§Book3§Sheet1§TableFoobar2</t>
+  </si>
+  <si>
+    <t>PreviousID</t>
+  </si>
+  <si>
+    <t>5A86F601F791F37D70A1A3B8FEDEB7BF2C7B88D4</t>
+  </si>
+  <si>
+    <t>00BF313399C32EE1563AC7BD598236C359126679</t>
+  </si>
+  <si>
+    <t>4C90630588DA709A3007B7EE0FB7DDFD9159BE90</t>
+  </si>
+  <si>
+    <t>135EC372181380110551F971B7FA0C4703A3739F</t>
+  </si>
+  <si>
+    <t>3028B7A9A3B110C6AA6640127F96D3310E5137D4</t>
+  </si>
+  <si>
+    <t>00D3E1214778099D4FA23326203B06AC6E46DC43</t>
+  </si>
+  <si>
+    <t>9598AED755869D9DE18753D2B2B0966604B1B825</t>
+  </si>
+  <si>
+    <t>00DE27E4B7421EC9E52AD33D82AFA4855B8DC64D</t>
   </si>
 </sst>
 </file>
@@ -1883,9 +1911,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S29" sqref="S29"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1909,9 +1935,7 @@
   </sheetPr>
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2463,9 +2487,7 @@
   </sheetPr>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2742,9 +2764,7 @@
   </sheetPr>
   <dimension ref="A1:I163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7090,6 +7110,144 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B57E1990-6657-4446-A9D2-4BB07C17F583}">
+  <sheetPr codeName="Sheet8">
+    <tabColor rgb="FFFF5050"/>
+  </sheetPr>
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="D2">
+        <v>70812</v>
+      </c>
+      <c r="E2" t="s">
+        <v>469</v>
+      </c>
+      <c r="F2" s="5">
+        <v>46012.915267939818</v>
+      </c>
+      <c r="G2" s="5">
+        <v>46012.915267939818</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="D3">
+        <v>95334</v>
+      </c>
+      <c r="E3" t="s">
+        <v>473</v>
+      </c>
+      <c r="F3" s="5">
+        <v>46012.915267824072</v>
+      </c>
+      <c r="G3" s="5">
+        <v>46012.915267824072</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="D4">
+        <v>54771</v>
+      </c>
+      <c r="E4" t="s">
+        <v>475</v>
+      </c>
+      <c r="F4" s="5">
+        <v>46012.915268171295</v>
+      </c>
+      <c r="G4" s="5">
+        <v>46012.915268171295</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4014D7D9-67F4-4F07-83FC-10C2F1BBCE3E}">
   <sheetPr codeName="Sheet5">
     <tabColor rgb="FFFF5050"/>
@@ -7974,16 +8132,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4456FD79-7C10-4AC5-BE66-AC86E4F74AB8}">
   <sheetPr codeName="Sheet4">
     <tabColor rgb="FFFF5050"/>
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8180,16 +8336,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21F1CC0D-2E2E-420C-91BE-F02116333066}">
   <sheetPr codeName="Sheet6">
     <tabColor rgb="FFFF5050"/>
   </sheetPr>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>